<commit_message>
Run mode changes mark as Yes and No and Excel Data updated with new Oauth changes
</commit_message>
<xml_diff>
--- a/DolphinApiTest/src/test/resources/SIT_TESTDATA.xlsx
+++ b/DolphinApiTest/src/test/resources/SIT_TESTDATA.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="47">
   <si>
     <t xml:space="preserve">Test_Case</t>
   </si>
@@ -65,63 +65,117 @@
     <t xml:space="preserve">TC_001_Send The Valid Request</t>
   </si>
   <si>
-    <t xml:space="preserve">Y</t>
+    <t xml:space="preserve">Yes</t>
   </si>
   <si>
     <t xml:space="preserve">/developer/auth-token </t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">{
+    "metadata": {
+        "X-App-ID": "IBPS",
+        "X-Correlation-ID": "31873127329799381273192"
+    },
+    "payload": {
+        "password": "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">SWJwc0AxMjM=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">",
+        "username": "ibps"
+    }
+}</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">X-Client-Id:53jt873l753mcudrhqmuh3g5u8,X-api-key:DTUDHv9UVG8cVT3qmhiSv1UcnvCduzLf1CI6zCVY</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">{
+    "username":"ibps",
+     "password":"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">SWJwc0AxMjM=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">"
+  }</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">payload</t>
+  </si>
+  <si>
+    <t xml:space="preserve">token</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Success</t>
+  </si>
+  <si>
+    <t xml:space="preserve">msgInfo.msgCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User Token generated successfully </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_002_Send The Request With Invalid Input Parameter</t>
+  </si>
+  <si>
     <t xml:space="preserve">{
-  "metadata":{
-    "appId":"IBPS",
-    "soaCorrelationId":"12221222211"
-  },
-  "payload":{
-    "username":"ibps",
-    "password":"Ibps@123"
-  }
-}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X-Client-Id:53jt873l753mcudrhqmuh3g5u8,X-api-key:DTUDHv9UVG8cVT3qmhiSv1UcnvCduzLf1CI6zCVY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{
-    "username":"ibps",
-     "password":"Ibps@123"
-  }</t>
-  </si>
-  <si>
-    <t xml:space="preserve">200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">payload</t>
-  </si>
-  <si>
-    <t xml:space="preserve">token</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Success</t>
-  </si>
-  <si>
-    <t xml:space="preserve">msgInfo.msgCode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User Token generated successfully </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_002_Send The Request With Invalid Input Parameter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{
-  "metadata":{
-    "appId":"IBPS",
-    "soaCorrelationId":"12221222211"
-  },
-  "payload":{
-    "username":"Username",
-    "password":"Password"
-  }
+    "metadata": {
+        "X-App-ID": "IBPS",
+        "X-Correlation-ID": "31873127329799381273192"
+    },
+    "payload": {
+        "password": "",
+        "username": ""
+    }
 }</t>
   </si>
   <si>
@@ -145,9 +199,6 @@
   </si>
   <si>
     <t xml:space="preserve">TC_003_Send The Request with Empty Client ID </t>
-  </si>
-  <si>
-    <t xml:space="preserve">y</t>
   </si>
   <si>
     <t xml:space="preserve">X-api-key:DTUDHv9UVG8cVT3qmhiSv1UcnvCduzLf1CI6zCVY</t>
@@ -244,7 +295,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -272,6 +323,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u val="single"/>
@@ -404,35 +461,35 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -516,7 +573,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -524,7 +581,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="36.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="27.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25.14"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.52"/>
@@ -578,7 +635,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="237.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="131.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -619,7 +676,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="237.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="131.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>25</v>
       </c>
@@ -629,7 +686,7 @@
       <c r="C3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="5" t="s">
         <v>26</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -660,21 +717,21 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="237.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="131.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="5" t="s">
         <v>26</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>18</v>
@@ -692,19 +749,18 @@
         <v>22</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L4" s="13" t="s">
         <v>23</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="{&#10;&#10;  &quot;metadata&quot;:{&#10;&#10;    &quot;appId&quot;:&quot;IBPS&quot;,&#10;&#10;    &quot;soaCorrelationId&quot;:&quot;12221222211&quot;&#10;&#10;  },&#10;&#10;  &quot;payload&quot;:{&#10;&#10;    &quot;username&quot;:&quot;ibps&quot;,&#10;&#10;    &quot;password&quot;:&quot;Ibps@123&quot;&#10;&#10;  }&#10;&#10;}"/>
-    <hyperlink ref="F3" r:id="rId2" display="{&#10;    &quot;username&quot;:&quot;ibps&quot;,&#10;     &quot;password&quot;:&quot;Ibps@1234&quot;&#10;&#10;  }"/>
+    <hyperlink ref="F3" r:id="rId1" display="{&#10;    &quot;username&quot;:&quot;ibps&quot;,&#10;     &quot;password&quot;:&quot;Ibps@1234&quot;&#10;&#10;  }"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -723,8 +779,8 @@
   </sheetPr>
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -757,13 +813,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>9</v>
@@ -771,22 +827,22 @@
     </row>
     <row r="2" customFormat="false" ht="213.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>19</v>
@@ -795,27 +851,27 @@
         <v>20</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="127.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>43</v>
-      </c>
       <c r="F3" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>19</v>
@@ -824,7 +880,7 @@
         <v>20</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes in LE service specification factory excel file
</commit_message>
<xml_diff>
--- a/DolphinApiTest/src/test/resources/SIT_TESTDATA.xlsx
+++ b/DolphinApiTest/src/test/resources/SIT_TESTDATA.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="48">
   <si>
     <t xml:space="preserve">Test_Case</t>
   </si>
@@ -71,44 +71,16 @@
     <t xml:space="preserve">/developer/auth-token </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">{
+    <t xml:space="preserve">{
     "metadata": {
         "X-App-ID": "IBPS",
         "X-Correlation-ID": "31873127329799381273192"
     },
     "payload": {
-        "password": "</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">SWJwc0AxMjM=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">",
+        "password": "SWJwc0AxMjM=",
         "username": "ibps"
     }
 }</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">X-Client-Id:53jt873l753mcudrhqmuh3g5u8,X-api-key:DTUDHv9UVG8cVT3qmhiSv1UcnvCduzLf1CI6zCVY</t>
@@ -131,6 +103,7 @@
         <color rgb="FF0000FF"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">SWJwc0AxMjM=</t>
     </r>
@@ -283,6 +256,9 @@
     <t xml:space="preserve">TC_002_Send the Invalid request</t>
   </si>
   <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
     <t xml:space="preserve">   {
    	"ageOfPayer": " "
    }</t>
@@ -295,7 +271,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -323,12 +299,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <u val="single"/>
@@ -461,35 +431,35 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -779,8 +749,8 @@
   </sheetPr>
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -859,7 +829,7 @@
         <v>45</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>40</v>
@@ -871,7 +841,7 @@
         <v>42</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
name changes in reusable function url change in excel file
</commit_message>
<xml_diff>
--- a/DolphinApiTest/src/test/resources/SIT_TESTDATA.xlsx
+++ b/DolphinApiTest/src/test/resources/SIT_TESTDATA.xlsx
@@ -3,16 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{A494BADB-38AF-40D0-910D-FCB4B60DD8D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{8544F813-61C5-4F1A-832B-A108EA2F4348}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="16500" windowHeight="11820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="16530" windowHeight="11820" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TokenApiTest" sheetId="1" r:id="rId1"/>
     <sheet name="LE_FTSP" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="F3:L4"/>
+  <oleSize ref="A3:F14"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -797,9 +797,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I2" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
-    </sheetView>
+    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1000,8 +998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
JACOCO Modification and Editing
</commit_message>
<xml_diff>
--- a/DolphinApiTest/src/test/resources/SIT_TESTDATA.xlsx
+++ b/DolphinApiTest/src/test/resources/SIT_TESTDATA.xlsx
@@ -3,16 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{A494BADB-38AF-40D0-910D-FCB4B60DD8D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{AA1EF7B7-5E66-4652-B1C1-B5BCFBEDC17F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="16500" windowHeight="11820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="16530" windowHeight="11820" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TokenApiTest" sheetId="1" r:id="rId1"/>
     <sheet name="LE_FTSP" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="F3:L4"/>
+  <oleSize ref="A3:F14"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -797,8 +797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I2" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView topLeftCell="A4" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1000,8 +1000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>